<commit_message>
State after discussed sampsize calculation
</commit_message>
<xml_diff>
--- a/inst/extdata/2024.12.21/t1t0.xlsx
+++ b/inst/extdata/2024.12.21/t1t0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c770e11f011a8c48/DKM/Válallkozás/TMC_Personal/Papp Marci AB ICU/TMC.PappMarciAB/inst/extdata/2024.12.21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14EED7AD-9734-473D-8657-A0EA27E86B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{14EED7AD-9734-473D-8657-A0EA27E86B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD34647E-D306-49CA-984A-8E27BBBC4FD7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4464899B-8F0D-4149-B452-3448341315CE}"/>
   </bookViews>
@@ -203,10 +203,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -546,7 +546,7 @@
   <dimension ref="A1:F115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>